<commit_message>
primeros cambios realizados por Julio en Capital semilla
</commit_message>
<xml_diff>
--- a/Mi Inventario Amway.xlsx
+++ b/Mi Inventario Amway.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Angel\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="9240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Productos!$A$1:$H$127</definedName>
     <definedName name="lista">Productos!$A$2:$H$127</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -960,8 +955,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1489,7 +1484,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1506,11 +1501,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1523,7 +1518,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1540,7 +1535,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1553,7 +1548,7 @@
     <xf numFmtId="4" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1574,7 +1569,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1619,7 +1614,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1661,10 +1656,10 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="8" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1825,7 +1820,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1860,7 +1855,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2037,7 +2032,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2047,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD127"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6989,8 +6984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8030,8 +8025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9031,7 +9026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -10001,8 +9996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10059,7 +10054,7 @@
       </c>
       <c r="J5" s="107"/>
       <c r="K5" s="39">
-        <f>IF(AND(C3="x",D3="",E3=""),'Mi Negocio'!H32,IF(AND('Capital Semilla'!D3="x",'Capital Semilla'!C3="",'Capital Semilla'!E3=""),'Socio 1'!#REF!,0))</f>
+        <f>IF(AND(C3="x",D3="",E3=""),'Mi Negocio'!H32,IF(AND('Capital Semilla'!D3="x",'Capital Semilla'!C3="",'Capital Semilla'!E3=""),'Socio 1'!H32,0))</f>
         <v>156038.49985310147</v>
       </c>
     </row>
@@ -10099,15 +10094,15 @@
         <v>281</v>
       </c>
       <c r="C7" s="60">
-        <f>IF(A7="x",$K$6,IF(#REF!&lt;&gt;0,(#REF!-$L$9)*$K$9/$I$3,""))</f>
+        <f>IF(A7="x",$K$6,IF(K5&lt;&gt;0,K6,""))</f>
         <v>334.08</v>
       </c>
       <c r="D7" s="66">
-        <f>IF(A7="x",$K$5,IF(D4&lt;&gt;"",(F6*$K$9)-$L$9,""))</f>
+        <f>IF(A7="x",$K$5,IF(C7&lt;&gt;"",(K5*$K$9)-$L$9,""))</f>
         <v>156038.49985310147</v>
       </c>
       <c r="E7" s="66">
-        <f>IF(A7="x",$K$7,IF(D6&lt;&gt;"",D7*42.857143%,""))</f>
+        <f>IF(A7="x",$K$7,IF(D7&lt;&gt;"",D7*42.857143%,""))</f>
         <v>64016.500146898528</v>
       </c>
       <c r="F7" s="66">
@@ -10133,7 +10128,7 @@
         <v>1041.2289156626507</v>
       </c>
       <c r="D8" s="67">
-        <f>IF(A8="x",$K$5,IF(D6&lt;&gt;"",(F7*$K$9)-$L$9,""))</f>
+        <f>IF(A8="x",$K$5,IF(D7&lt;&gt;"",(F7*$K$9)-$L$9,""))</f>
         <v>436110</v>
       </c>
       <c r="E8" s="67">
@@ -10155,7 +10150,7 @@
         <v>2983.2013799387951</v>
       </c>
       <c r="D9" s="67">
-        <f t="shared" ref="D9:D18" si="2">IF(A9="x",$K$5,IF(D7&lt;&gt;"",(F8*$K$9)-$L$9,""))</f>
+        <f t="shared" ref="D9:D18" si="2">IF(A9="x",$K$5,IF(D8&lt;&gt;"",(F8*$K$9)-$L$9,""))</f>
         <v>1242028.5726745999</v>
       </c>
       <c r="E9" s="67">

</xml_diff>